<commit_message>
Added a draft SRS to fulfill review points.
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/PO3_DGW_SRS_Review.xlsx
+++ b/Software Specification/SRS/PO3_DGW_SRS_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E75956-49FF-4BF6-A34D-E90F0DCC7B83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -542,12 +543,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -559,43 +590,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -933,10 +934,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -947,189 +948,206 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31">
+      <c r="C7" s="33"/>
+      <c r="D7" s="25">
         <v>1</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1146,23 +1164,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1170,11 +1171,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,7 +1239,9 @@
       <c r="F2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
@@ -1263,7 +1266,9 @@
       <c r="F3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
@@ -1291,7 +1296,9 @@
       <c r="F4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
@@ -1835,10 +1842,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$3:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$6:$K$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixed SRS requirement organization to be compatible with CYRS V0.4
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/PO3_DGW_SRS_Review.xlsx
+++ b/Software Specification/SRS/PO3_DGW_SRS_Review.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E75956-49FF-4BF6-A34D-E90F0DCC7B83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295063E4-ED08-4023-ABC5-018845006D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -543,12 +543,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -563,33 +590,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -948,206 +948,189 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="40"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="25">
+      <c r="C7" s="26"/>
+      <c r="D7" s="31">
         <v>1</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="36"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1164,6 +1147,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1326,9 @@
       <c r="F5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>19</v>
       </c>
@@ -1351,7 +1353,9 @@
       <c r="F6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
@@ -1369,7 +1373,9 @@
       <c r="F7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Update SRS reveiw sheet with resoled ppoints
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/PO3_DGW_SRS_Review.xlsx
+++ b/Software Specification/SRS/PO3_DGW_SRS_Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295063E4-ED08-4023-ABC5-018845006D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -171,11 +170,17 @@
   <si>
     <t>31/01/2020</t>
   </si>
+  <si>
+    <t>23/2/2020</t>
+  </si>
+  <si>
+    <t>Update resolved points</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -543,12 +548,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -560,43 +595,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -934,203 +939,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25" t="s">
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="32"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1147,23 +1177,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1171,27 +1184,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
@@ -1243,11 +1256,11 @@
         <v>20</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>44</v>
       </c>
@@ -1270,14 +1283,14 @@
         <v>20</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I3" s="10"/>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
@@ -1300,14 +1313,14 @@
         <v>20</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I4" s="10"/>
       <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>44</v>
       </c>
@@ -1330,11 +1343,11 @@
         <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>44</v>
       </c>
@@ -1357,14 +1370,14 @@
         <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I6" s="12"/>
       <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -1377,14 +1390,14 @@
         <v>20</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I7" s="12"/>
       <c r="K7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13"/>
@@ -1392,12 +1405,10 @@
       <c r="E8" s="24"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="H8" s="10"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
@@ -1408,7 +1419,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1425,7 +1436,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1442,7 +1453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1453,7 +1464,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1464,7 +1475,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1475,7 +1486,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1486,7 +1497,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1497,7 +1508,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1508,7 +1519,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1519,7 +1530,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1530,7 +1541,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1541,7 +1552,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1552,7 +1563,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1563,7 +1574,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1574,7 +1585,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1585,7 +1596,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1596,7 +1607,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1607,7 +1618,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1618,7 +1629,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1629,7 +1640,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1640,7 +1651,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1651,7 +1662,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1662,7 +1673,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1673,7 +1684,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1684,7 +1695,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1695,7 +1706,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1706,7 +1717,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1717,7 +1728,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1728,7 +1739,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1739,7 +1750,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1750,7 +1761,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1761,7 +1772,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1772,7 +1783,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1783,7 +1794,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1794,7 +1805,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1805,7 +1816,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1816,7 +1827,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -1848,10 +1859,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>$K$3:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$6:$K$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>